<commit_message>
formats Vadkarok HR to GSheet specification
</commit_message>
<xml_diff>
--- a/data/szekelyhon_data.xlsx
+++ b/data/szekelyhon_data.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Skydrive\Github\szekelydata\medveterkep\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F015018-881B-40DA-A405-EEA6A6AD3A38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="95">
   <si>
     <t>date</t>
   </si>
@@ -31,6 +25,9 @@
     <t>image</t>
   </si>
   <si>
+    <t>source</t>
+  </si>
+  <si>
     <t>title</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
     <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2018/06_julius/sm_medvecsapda-3-ba-3.jpg</t>
   </si>
   <si>
+    <t>Székelyhon</t>
+  </si>
+  <si>
     <t>Még a rókák is kerülik az Udvarhelyhez közeli üregbe húzódott bocsos anyamedvét</t>
   </si>
   <si>
@@ -229,7 +229,7 @@
     <t>Egyedül bóklászó egyéves medvebocsot gázolt el egy autó péntekre virradóan Újszékely határában. A vadállat az ütközést követően elpusztult – számol be a Hargita megyei önkormányzat sajtóirodája.</t>
   </si>
   <si>
-    <t>Ismét medvebiztos szeméttárolóba rekedt egy bocs szerdára virradóan a tusnádfürdői vasútállomás közelében. A vadállatot a Hargita megyei csendőrök szabadították ki, miután az anyamedvét többször is elriasztották a helyszínről. </t>
+    <t xml:space="preserve">Ismét medvebiztos szeméttárolóba rekedt egy bocs szerdára virradóan a tusnádfürdői vasútállomás közelében. A vadállatot a Hargita megyei csendőrök szabadították ki, miután az anyamedvét többször is elriasztották a helyszínről. </t>
   </si>
   <si>
     <t>A Ro-Alert riasztórendszeren keresztül figyelmeztették szerdán reggel a hatóságok a sepsiszentgyörgyieket, hogy medve kószál a városban.</t>
@@ -256,7 +256,7 @@
     <t>Villanypásztort szereltek fel a Csíkszeredai Megyei Sürgősségi Kórház körül húzódó kerítésre kedden. Az eszköz az intézmény területére korábban több alkalommal behatoló medvéket hivatott távol tartani.</t>
   </si>
   <si>
-    <t>A napokban hoz döntést a kőrispataki medvetámadás miatt félárván maradt két kiskorú elhelyezéséről a Hargita Megyei Szociális és Gyermekvédelmi Igazgatóság. </t>
+    <t xml:space="preserve">A napokban hoz döntést a kőrispataki medvetámadás miatt félárván maradt két kiskorú elhelyezéséről a Hargita Megyei Szociális és Gyermekvédelmi Igazgatóság. </t>
   </si>
   <si>
     <t>Videót készített a kőrispataki medvéről, a barlangjáról és a pénteki medvetámadás helyszínéről a Hubertus Vadásztársaság igazgatója. A felvétel azonban hamar megszakad, ugyanis az állat a köztük lévő mély árkot megkerülve a vadászok felé rohan.</t>
@@ -304,11 +304,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,14 +385,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -439,7 +431,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,27 +463,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -523,24 +497,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -716,21 +672,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:N19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -771,29 +722,32 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1"/>
       <c r="B2" s="2">
         <v>43530</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -801,125 +755,134 @@
       <c r="J2">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>87</v>
       </c>
       <c r="M2">
-        <v>46.304999600000002</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>25.292647899999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>46.3049996</v>
+      </c>
+      <c r="O2">
+        <v>25.2926479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1"/>
       <c r="B3" s="2">
         <v>43540</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>88</v>
       </c>
       <c r="M3">
-        <v>46.260836599999998</v>
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>24.973189399999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>46.2608366</v>
+      </c>
+      <c r="O3">
+        <v>24.9731894</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1"/>
       <c r="B4" s="2">
         <v>43544</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
-        <v>87</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>89</v>
       </c>
       <c r="M4">
-        <v>46.146075199999999</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>25.856958899999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>46.1460752</v>
+      </c>
+      <c r="O4">
+        <v>25.8569589</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
         <v>43544</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -927,83 +890,89 @@
       <c r="J5">
         <v>0</v>
       </c>
-      <c r="K5" t="s">
-        <v>88</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>90</v>
       </c>
       <c r="M5">
-        <v>45.860937499999999</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>25.788579599999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>45.8609375</v>
+      </c>
+      <c r="O5">
+        <v>25.7885796</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>43546</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
+        <v>73</v>
       </c>
       <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>3</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
       <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>89</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>91</v>
       </c>
       <c r="M6">
-        <v>46.417812300000001</v>
+        <v>0</v>
       </c>
       <c r="N6">
+        <v>46.4178123</v>
+      </c>
+      <c r="O6">
         <v>24.9703704</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="1"/>
       <c r="B7" s="2">
         <v>43547</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1011,41 +980,44 @@
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7" t="s">
-        <v>89</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>91</v>
       </c>
       <c r="M7">
-        <v>46.417812300000001</v>
+        <v>0</v>
       </c>
       <c r="N7">
+        <v>46.4178123</v>
+      </c>
+      <c r="O7">
         <v>24.9703704</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
         <v>43549</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1053,41 +1025,44 @@
       <c r="J8">
         <v>0</v>
       </c>
-      <c r="K8" t="s">
-        <v>89</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>91</v>
       </c>
       <c r="M8">
-        <v>46.417812300000001</v>
+        <v>0</v>
       </c>
       <c r="N8">
+        <v>46.4178123</v>
+      </c>
+      <c r="O8">
         <v>24.9703704</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="1"/>
       <c r="B9" s="2">
         <v>43550</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1095,41 +1070,44 @@
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9" t="s">
-        <v>89</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>91</v>
       </c>
       <c r="M9">
-        <v>46.417812300000001</v>
+        <v>0</v>
       </c>
       <c r="N9">
+        <v>46.4178123</v>
+      </c>
+      <c r="O9">
         <v>24.9703704</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="1"/>
       <c r="B10" s="2">
         <v>43550</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1137,41 +1115,44 @@
       <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10" t="s">
-        <v>88</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" t="s">
+        <v>90</v>
       </c>
       <c r="M10">
-        <v>45.860937499999999</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>25.788579599999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>45.8609375</v>
+      </c>
+      <c r="O10">
+        <v>25.7885796</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>43551</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1179,41 +1160,44 @@
       <c r="J11">
         <v>0</v>
       </c>
-      <c r="K11" t="s">
-        <v>89</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>91</v>
       </c>
       <c r="M11">
-        <v>46.417812300000001</v>
+        <v>0</v>
       </c>
       <c r="N11">
+        <v>46.4178123</v>
+      </c>
+      <c r="O11">
         <v>24.9703704</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="1"/>
       <c r="B12" s="2">
         <v>43551</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
+        <v>79</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1221,41 +1205,44 @@
       <c r="J12">
         <v>0</v>
       </c>
-      <c r="K12" t="s">
-        <v>90</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12" t="s">
+        <v>92</v>
       </c>
       <c r="M12">
-        <v>46.369557399999998</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>25.795365499999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>46.3695574</v>
+      </c>
+      <c r="O12">
+        <v>25.7953655</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1"/>
       <c r="B13" s="2">
         <v>43551</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
+        <v>80</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1263,83 +1250,89 @@
       <c r="J13">
         <v>0</v>
       </c>
-      <c r="K13" t="s">
-        <v>89</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>91</v>
       </c>
       <c r="M13">
-        <v>46.417812300000001</v>
+        <v>0</v>
       </c>
       <c r="N13">
+        <v>46.4178123</v>
+      </c>
+      <c r="O13">
         <v>24.9703704</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" s="1"/>
       <c r="B14" s="2">
         <v>43551</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>81</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
-      <c r="K14" t="s">
-        <v>89</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>91</v>
       </c>
       <c r="M14">
-        <v>46.417812300000001</v>
+        <v>0</v>
       </c>
       <c r="N14">
+        <v>46.4178123</v>
+      </c>
+      <c r="O14">
         <v>24.9703704</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15" s="1"/>
       <c r="B15" s="2">
         <v>43551</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="G15" t="s">
+        <v>82</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1347,32 +1340,35 @@
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="B16" s="2">
         <v>43554</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="G16" t="s">
+        <v>83</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1380,32 +1376,35 @@
       <c r="J16">
         <v>0</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1"/>
       <c r="B17" s="2">
         <v>43561</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="G17" t="s">
+        <v>84</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1413,83 +1412,89 @@
       <c r="J17">
         <v>0</v>
       </c>
-      <c r="K17" t="s">
-        <v>91</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>93</v>
       </c>
       <c r="M17">
-        <v>46.853258099999998</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>24.819102900000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <v>46.8532581</v>
+      </c>
+      <c r="O17">
+        <v>24.8191029</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1"/>
       <c r="B18" s="2">
         <v>43562</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="G18" t="s">
+        <v>85</v>
       </c>
       <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>2</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>14</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18" t="s">
-        <v>92</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>94</v>
       </c>
       <c r="M18">
-        <v>46.334716999999998</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>25.009115600000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>46.334717</v>
+      </c>
+      <c r="O18">
+        <v>25.0091156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1"/>
       <c r="B19" s="2">
         <v>43572</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>86</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1497,59 +1502,61 @@
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>87</v>
       </c>
       <c r="M19">
-        <v>46.304999600000002</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>25.292647899999999</v>
+        <v>46.3049996</v>
+      </c>
+      <c r="O19">
+        <v>25.2926479</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="C11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="C12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D12" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C14" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="C15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D15" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C16" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="C17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D17" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="C18" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="C19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D19" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="D4" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId7"/>
+    <hyperlink ref="D5" r:id="rId8"/>
+    <hyperlink ref="C6" r:id="rId9"/>
+    <hyperlink ref="D6" r:id="rId10"/>
+    <hyperlink ref="C7" r:id="rId11"/>
+    <hyperlink ref="D7" r:id="rId12"/>
+    <hyperlink ref="C8" r:id="rId13"/>
+    <hyperlink ref="D8" r:id="rId14"/>
+    <hyperlink ref="C9" r:id="rId15"/>
+    <hyperlink ref="D9" r:id="rId16"/>
+    <hyperlink ref="C10" r:id="rId17"/>
+    <hyperlink ref="D10" r:id="rId18"/>
+    <hyperlink ref="C11" r:id="rId19"/>
+    <hyperlink ref="D11" r:id="rId20"/>
+    <hyperlink ref="C12" r:id="rId21"/>
+    <hyperlink ref="D12" r:id="rId22"/>
+    <hyperlink ref="C13" r:id="rId23"/>
+    <hyperlink ref="D13" r:id="rId24"/>
+    <hyperlink ref="C14" r:id="rId25"/>
+    <hyperlink ref="D14" r:id="rId26"/>
+    <hyperlink ref="C15" r:id="rId27"/>
+    <hyperlink ref="D15" r:id="rId28"/>
+    <hyperlink ref="C16" r:id="rId29"/>
+    <hyperlink ref="D16" r:id="rId30"/>
+    <hyperlink ref="C17" r:id="rId31"/>
+    <hyperlink ref="D17" r:id="rId32"/>
+    <hyperlink ref="C18" r:id="rId33"/>
+    <hyperlink ref="D18" r:id="rId34"/>
+    <hyperlink ref="C19" r:id="rId35"/>
+    <hyperlink ref="D19" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updtes january 2020 data, fixes vadkarok missing dates
</commit_message>
<xml_diff>
--- a/data/szekelyhon_data.xlsx
+++ b/data/szekelyhon_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Github\szekelydata\medveterkep\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C65D1D-29B7-43B7-91E3-02E2E80E3192}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2AB913-5B65-4EAF-8158-98A1B6452CE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>date</t>
   </si>
@@ -67,136 +67,154 @@
     <t>checked</t>
   </si>
   <si>
-    <t>https://szekelyhon.ro/aktualis/medveproblema-brusszeli-nyomasgyakorlasban-biznak-a-szekelyfoldi-megyek-vezetoi</t>
-  </si>
-  <si>
-    <t>https://szekelyhon.ro/aktualis/sokkos-allapotban-kerult-korhazba-a-medvetamadas-aldozata</t>
-  </si>
-  <si>
-    <t>https://szekelyhon.ro/aktualis/kilonek-a-hidegkuton-emberre-tamado-medvet</t>
-  </si>
-  <si>
-    <t>https://szekelyhon.ro/aktualis/szeben-es-feher-megye-is-csatlakozott-a-bmedvepeticiohozr</t>
-  </si>
-  <si>
-    <t>https://szekelyhon.ro/aktualis/megteritik-a-gazdaknak-az-elmult-harom-evben-tortent-medvekarokat</t>
-  </si>
-  <si>
-    <t>https://szekelyhon.ro/aktualis/csiksomlyon-jar-a-medve-n-figyelmeztet-a-ro-alert</t>
-  </si>
-  <si>
-    <t>https://szekelyhon.ro/aktualis/kilottek-a-medvet-amely-majus-ota-tartotta-rettegesben-a-specialis-iskola-tanuloit</t>
-  </si>
-  <si>
-    <t>https://szekelyhon.ro/aktualis/szamitani-kell-arra-hogy-telen-is-aktivak-lehetnek-a-medvek</t>
-  </si>
-  <si>
-    <t>https://szekelyhon.ro/aktualis/a-haztaji-gazdasagban-levo-osszes-birkat-megolte-a-medve-gyergyovaslabon</t>
-  </si>
-  <si>
-    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2017/05_augusztus/01/sm_medve-cekend-ba-5.jpg</t>
-  </si>
-  <si>
-    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2018/06_julius/sm_egeszsegugy-vn-048.jpg</t>
-  </si>
-  <si>
-    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2018/08_majus/01/sm_medve-kiloves-remete-ba-5.jpg</t>
-  </si>
-  <si>
-    <t>https://media.szekelyhon.ro/pictures/csik/aktualis/2019/06_julius/sm_kukazomedvek-tusnadfurdo-pnt-4.jpg</t>
-  </si>
-  <si>
-    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2019/03_oktober/03/sm_medvetamadas_belo-4.jpg</t>
-  </si>
-  <si>
-    <t>https://media.szekelyhon.ro/pictures/csik/aktualis/2019/01_december/sm_ro-alert-somlyo01.jpg</t>
-  </si>
-  <si>
-    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2018/08_majus/01/sm_medve-kiloves-remete-ba-13.jpg</t>
+    <t>https://szekelyhon.ro/aktualis/feldulva-talaltak-a-sirhelyeket</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/elutasitotta-medveugyben-a-zetelaki-terulettulajdonosi-tarsulas-keresetet-a-tablabirosag</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/ki-akadalyozta-meg-hogy-a-barnamedve-lekeruljon-a-szigoruan-vedett-allatfajok-listajarol-romaniaban</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/penzt-iger-a-miniszter-a-medvek-altal-veszelyeztetett-telepulesek-vedelmere</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/hargita-megye-megvan-az-ev-elso-112-s-medveeszlelese</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/aktivak-a-medvek-szekelyudvarhely-kornyeken</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/lemondott-a-vadasztarsasag-az-emberre-tamado-hidegkuti-medve-kiloveserol</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/szagra-jonnek-a-medvek</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/medveradar-zetelakan-es-farkaslakan-voltak-a-legaktivabbak-tavaly-a-nagyvadak</t>
+  </si>
+  <si>
+    <t>https://szekelyhon.ro/aktualis/gyergyoszentmiklos-utcain-koborolt-egy-medve</t>
+  </si>
+  <si>
+    <t>https://media.szekelyhon.ro/pictures/agerpres/kiemelesek/10_kiemelesek/sm_feldult-temeto-vaslab-9.jpg</t>
+  </si>
+  <si>
+    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2018/12_januar/01/sm_medvek-pa-18.jpg</t>
+  </si>
+  <si>
+    <t>https://media.szekelyhon.ro/pictures/csik/aktualis/2019/06_julius/sm_kukazomedvek-tusnadfurdo-pnt.jpg</t>
+  </si>
+  <si>
+    <t>https://media.szekelyhon.ro/pictures/csik/aktualis/2019/07_junius/02/sm_kukazomedve-tusnadfurdo-pnt-3.jpg</t>
+  </si>
+  <si>
+    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2019/03_oktober/03/sm_medve-elutottek-ebe-3.jpg</t>
+  </si>
+  <si>
+    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2018/12_januar/01/sm_medvek-pa-8.jpg</t>
+  </si>
+  <si>
+    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2016/12_januar/sm_medvebarlang-ab-1.jpg</t>
+  </si>
+  <si>
+    <t>https://media.szekelyhon.ro/pictures/csik/aktualis/2019/06_julius/sm_kukazomedvek-tusnadfurdo-pnt-12.jpg</t>
   </si>
   <si>
     <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2018/12_januar/01/sm_medvek-pa-24.jpg</t>
   </si>
   <si>
-    <t>https://media.szekelyhon.ro/pictures/udvarhely/aktualis/2015/03_oktober/sm_farkastamadas-felsoboldogfalva-ab-76.jpg</t>
+    <t>https://media.szekelyhon.ro/pictures/csik/aktualis/2013/12_januar/sm_medvek_kr_10.jpg</t>
   </si>
   <si>
     <t>Székelyhon</t>
   </si>
   <si>
-    <t>Medveprobléma: brüsszeli nyomásgyakorlásban bíznak a székelyföldi megyék vezetői</t>
-  </si>
-  <si>
-    <t>Sokkos állapotban került kórházba a medvetámadás áldozata</t>
-  </si>
-  <si>
-    <t>Kilőnék a Hidegkúton emberre támadó medvét</t>
-  </si>
-  <si>
-    <t>Szeben és Fehér megye is csatlakozott a „medvepetícióhoz”</t>
-  </si>
-  <si>
-    <t>Megtérítik a gazdáknak az elmúlt három évben történt medvekárokat</t>
-  </si>
-  <si>
-    <t>Csíksomlyón jár a medve – figyelmeztet a Ro-Alert</t>
-  </si>
-  <si>
-    <t>Kilőtték a medvét, amely május óta rettegésben tartotta a speciális iskola tanulóit</t>
-  </si>
-  <si>
-    <t>Számítani kell arra, hogy télen is aktívak lehetnek a medvék</t>
-  </si>
-  <si>
-    <t>A háztáji gazdaságban levő összes birkát megölte a medve Gyergyóvaslábon</t>
-  </si>
-  <si>
-    <t>Brüsszelben keresnek támogatást az egyre súlyosbodó medveproblémára Hargita, Kovászna, Maros és Brassó megye vezetői. Úgy vélik, „Bukarestben akkor kapják fel a fejüket, ha Brüsszelből kapnak egy intést”. </t>
-  </si>
-  <si>
-    <t>Mellkasi sérülései a legsúlyosabbak annak a férfinak, aki medvetámadásban szerzett többszöri zúzott sebeket testének gyomortájékán, az ágyéki részen és könyökén kedd este. Az elsődleges információk szerint a hidegkúti férfi az esztenáról tért haza, amikor saját kertjében rátámadt a nagyvad.</t>
-  </si>
-  <si>
-    <t>Kérni fogja az engedélyt a székelykeresztúri Hubertus Vadászegyesület a környezetvédelmi minisztériumtól azon medve kilövésére, amely kedden rátámadt egy férfire Hidegkúton.</t>
-  </si>
-  <si>
-    <t>Szeben és Fehér megyék vezetői is aláírták az Európai Parlament (EP) Petíciós Bizottságához benyújtandó folyamodványt, amelyben ismertetik, hogy az elszaporodott medveállomány veszélyezteti az emberéletet, és a mezőgazdasági javak sincsenek biztonságban.</t>
-  </si>
-  <si>
-    <t>Biztosítják az önkormányzatok működését az idei évre, kifizetik a Helyi Fejlesztési Országos Program támogatásait, és az elmúlt három év medvekárait is megtérítik a gazdáknak – jelentették be Csíkszeredában az RMDSZ politikusai a kormány által meghozott költségvetés-kiigazítást ismertetve.</t>
-  </si>
-  <si>
-    <t>Csíksomlyón, a sípálya környékén felbukkant medvéről kaptak bejelentést a hatóságok hétfő késődélután, a vészhelyzeti felügyelőség azonnal figyelmeztető üzenetet küldött a Ro-Alert rendszeren keresztül a környéken lévőknek.</t>
-  </si>
-  <si>
-    <t>Kilőtték hétvégén azt a medvét, amely május óta tartotta rettegésben az oltszemi speciális iskolában tanuló ötven, állami gondozásban lévő gyermeket, illetve gondozóikat.</t>
-  </si>
-  <si>
-    <t>Egyértelmű, hogy Székelyföldön még nem vonultak téli álomra a medvék, ezért arra voltunk kíváncsiak, hogy ez általában milyen körülmények között történik meg. A vadászok szerint az elkövetkező hónapokban is számíthatunk nagyvadak által okozott károkra.</t>
-  </si>
-  <si>
-    <t>Tizenegy birkát ölt meg a hétfőről keddre virradó éjszaka egy nőstény medve Gyergyóvasláb község egyik, vonatállomáshoz közeli házának udvarán.</t>
+    <t>Feldúlva találták a sírhelyeket</t>
+  </si>
+  <si>
+    <t>Elutasította medveügyben a Zetelaki Területtulajdonosi Társulás keresetét a táblabíróság</t>
+  </si>
+  <si>
+    <t>Ki akadályozta meg, hogy a barnamedve lekerüljön a szigorúan védett állatfajok listájáról Romániában?</t>
+  </si>
+  <si>
+    <t>Pénzt ígér a miniszter a medvék által veszélyeztetett települések védelmére</t>
+  </si>
+  <si>
+    <t>Hargita megye: megvan az év első 112-s medveészlelése</t>
+  </si>
+  <si>
+    <t>Aktívak a medvék Székelyudvarhely környékén</t>
+  </si>
+  <si>
+    <t>Lemondott a vadásztársaság az emberre támadó hidegkúti medve kilövéséről</t>
+  </si>
+  <si>
+    <t>Amíg elérhető közelségben van az ételmaradék, addig a medvék jelenlétére is számítani kell</t>
+  </si>
+  <si>
+    <t>Medveradar: Zetelakán és Farkaslakán voltak a legaktívabbak tavaly a nagyvadak</t>
+  </si>
+  <si>
+    <t>Gyergyószentmiklós utcáin kóborolt egy medve</t>
+  </si>
+  <si>
+    <t>Feldúlva találták a sírhelyeket, illetve azok környékét a Vasláb községhez tartozó hevederi temetőben. A nyomok alapján medvejárásra gyanakodnak.</t>
+  </si>
+  <si>
+    <t>Elutasította a Marosvásárhelyi Táblabíróság a Zetelaki Területtulajdonosi Társulás keresetét, amelyet a társulás a Környezetvédelmi Minisztérium ellen indított a vadgazdálkodási szabályozások alkalmazásának elmulasztása miatt. A társulás vezetője fellebbezést tervez.</t>
+  </si>
+  <si>
+    <t>Az állatvédők és az Európai Bizottság akadályozta meg, hogy a barnamedve öt évre lekerüljön a szigorúan védett állatfajok listájáról Romániában – állítja Benkő Erika RMDSZ-képviselő. </t>
+  </si>
+  <si>
+    <t>A háromszéki Zabolán tartott terepszemlét Costel Alexe környezetvédelmi miniszter, aki a látogatást követően arról számol be, hogy körvonalazódott egy olyan finanszírozási program, amely lehetővé teszi a medvék által veszélyeztetett települések védelmét.</t>
+  </si>
+  <si>
+    <t>Medvét látott a kertjében egy parajdi férfi a Sóhát utcában szombaton délután. A nagyvadat a gyümölcsfáknál fedezte fel, mintegy száz méterre a lakóháztól. Az esetet a 112-n jelentette, a helyszínre egy csendőri és egy mentőegység szállt ki.</t>
+  </si>
+  <si>
+    <t>Noha a magasabban fekvő térségekben már téli álmot alszanak a medvék, más területeken ez nem így van. Székelyudvarhely környékén például legalább tizenegy medve aktív jelenleg is, ezért a vadászok óvatosságra intenek.</t>
+  </si>
+  <si>
+    <t>Megúszta a kilövést a Hidegkúton emberre támadó medve, az illetékes vadásztársaságnál lemondtak arról, hogy a vad ártalmatlanítására rendkívüli jóváhagyást igényeljenek a környezetvédelmi minisztériumtól.</t>
+  </si>
+  <si>
+    <t>A szeméttárolók vonzzák a székelyudvarhelyi Cserehát lakónegyedbe az aktív nagyvadakat, ezért a Nagy-Küküllő Vadász- és Sporthorgász Egyesület medvebiztos kukákat rendelt, amelyeket a szemételszállító vállalattal egyeztetve helyezne ki. A medvék befogásával is próbálkoznak.</t>
+  </si>
+  <si>
+    <t>A kezdeti fellendülés után kissé lankadt az aktivitás a székelyföldi medveradar és -térkép néven emlegetett medveészlelő portálon, amelyet tavaly márciusban hozott létre Csala Dénes adatblogger. Ettől eltekintve a több mint 700 bejegyzést számláló medvetérkép a legszerteágazóbb adatbázisnak számít.</t>
+  </si>
+  <si>
+    <t>Egy városszéli üzemanyagtöltő állomásnál felbukkant medve miatt riasztották keddre virradóan a hatóságokat Gyergyószentmiklóson. Míg a csendőrök a nagyvadat kutatták, a vészhelyzeti felügyelőség a Ro-Alert rendszeren figyelmeztette a lakókat a veszélyre. A medvét végül megtalálták és elűzték.</t>
+  </si>
+  <si>
+    <t>Vasláb</t>
+  </si>
+  <si>
+    <t>Zetelaka</t>
+  </si>
+  <si>
+    <t>Sepsiszentgyörgy</t>
+  </si>
+  <si>
+    <t>Zabola</t>
+  </si>
+  <si>
+    <t>Parajd</t>
+  </si>
+  <si>
+    <t>Székelyudvarhely</t>
+  </si>
+  <si>
+    <t>Hidegkút</t>
   </si>
   <si>
     <t>Csíkszereda</t>
   </si>
   <si>
-    <t>Hidegkút</t>
-  </si>
-  <si>
-    <t>Székelykeresztúr</t>
-  </si>
-  <si>
-    <t>Szeben</t>
-  </si>
-  <si>
-    <t>Csíksomlyó</t>
-  </si>
-  <si>
-    <t>Oltszem</t>
-  </si>
-  <si>
-    <t>Vasláb</t>
+    <t>Gyergyószentmiklós</t>
   </si>
 </sst>
 </file>
@@ -615,15 +633,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A2" sqref="A2:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -676,28 +694,28 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2">
-        <v>43795</v>
+        <v>43824</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -706,43 +724,43 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>46.369557399999998</v>
+        <v>46.646074800000008</v>
       </c>
       <c r="O2">
-        <v>25.795365499999999</v>
+        <v>25.623710500000001</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2">
-        <v>43795</v>
+        <v>43825</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -751,37 +769,37 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>46.335918399999997</v>
+        <v>46.391030800000003</v>
       </c>
       <c r="O3">
-        <v>24.894142599999999</v>
+        <v>25.367929100000001</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2">
-        <v>43796</v>
+        <v>43834</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -796,37 +814,37 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>46.292452599999997</v>
+        <v>45.860937499999999</v>
       </c>
       <c r="O4">
-        <v>25.0317145</v>
+        <v>25.788579599999998</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2">
-        <v>43797</v>
+        <v>43836</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -841,37 +859,43 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M5">
         <v>0</v>
+      </c>
+      <c r="N5">
+        <v>45.887702999999988</v>
+      </c>
+      <c r="O5">
+        <v>26.189789000000001</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
-        <v>43798</v>
+        <v>43841</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -880,43 +904,43 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>46.369557399999998</v>
+        <v>46.555342899999999</v>
       </c>
       <c r="O6">
-        <v>25.795365499999999</v>
+        <v>25.127272300000001</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2">
-        <v>43801</v>
+        <v>43843</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -925,37 +949,37 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>46.3753277</v>
+        <v>46.304999600000002</v>
       </c>
       <c r="O7">
-        <v>25.819270299999999</v>
+        <v>25.292647899999999</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2">
-        <v>43801</v>
+        <v>43846</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -970,37 +994,37 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>45.970976</v>
+        <v>46.335918399999997</v>
       </c>
       <c r="O8">
-        <v>25.845801900000001</v>
+        <v>24.894142599999999</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2">
-        <v>43802</v>
+        <v>43851</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1014,53 +1038,107 @@
       <c r="K9">
         <v>0</v>
       </c>
+      <c r="L9" t="s">
+        <v>61</v>
+      </c>
       <c r="M9">
         <v>0</v>
+      </c>
+      <c r="N9">
+        <v>46.304999600000002</v>
+      </c>
+      <c r="O9">
+        <v>25.292647899999999</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2">
-        <v>43802</v>
+        <v>43856</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>46.646074800000008</v>
+        <v>46.369557399999998</v>
       </c>
       <c r="O10">
-        <v>25.623710500000001</v>
+        <v>25.795365499999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2">
+        <v>43858</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>64</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>46.721211199999999</v>
+      </c>
+      <c r="O11">
+        <v>25.585527500000001</v>
       </c>
     </row>
   </sheetData>
@@ -1083,8 +1161,10 @@
     <hyperlink ref="D9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="C10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="D10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>